<commit_message>
atualizar tasks no excell
</commit_message>
<xml_diff>
--- a/Anexos/pitstop_pro_taskboard.xlsx
+++ b/Anexos/pitstop_pro_taskboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kleman\OneDrive\Ambiente de Trabalho\Flag\Curso\Projecto\Pitstop-pro\Anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C19D91-2D26-47D2-8F27-F656176FED54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE72415-FDE0-4F61-95C8-62A5D2E014C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="52">
   <si>
     <t>Task</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Layout modular montado em Home.tsx</t>
   </si>
   <si>
-    <t>Tema dark com cores Tailwind personalizadas</t>
-  </si>
-  <si>
     <t>Estilização coerente com o tema nas páginas Register e Login</t>
   </si>
   <si>
@@ -161,6 +158,24 @@
   </si>
   <si>
     <t>Acessibilidade aplicada - ARIA's da vida</t>
+  </si>
+  <si>
+    <t>Criação de feature "Forgot My password" com recurso aos firebase errors</t>
+  </si>
+  <si>
+    <t>Dificuldade: após redefinir a pass fico "preso" numa página de redefinição que é gerida pelo firebase -há alguma forma simples de resolver?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> passagem geral para reforçar o uso de tipos em typescript</t>
+  </si>
+  <si>
+    <t>repensar e aprofundar para aplicar melhor TS no que já existe.</t>
+  </si>
+  <si>
+    <t>Planed</t>
+  </si>
+  <si>
+    <t>Tema inspirado nos sites de referência com cores Tailwind personalizadas</t>
   </si>
 </sst>
 </file>
@@ -189,7 +204,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,6 +232,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -261,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -285,6 +306,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,13 +613,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +632,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -617,42 +641,42 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="7"/>
     </row>
@@ -667,66 +691,66 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -740,319 +764,347 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
+      <c r="D20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="2"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
+      <c r="D26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="2"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>39</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
+      <c r="D33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="2"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="D37" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
+      <c r="C38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat(maintenance): cria página de manutenções com tabela editável
- Adiciona tipo Maintenance com os campos: data, descrição, veículo, KM e custo
- Cria tabela com inputs editáveis inline
- Integra página de manutenções com dados
</commit_message>
<xml_diff>
--- a/Anexos/pitstop_pro_taskboard.xlsx
+++ b/Anexos/pitstop_pro_taskboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kleman\OneDrive\Ambiente de Trabalho\Flag\Curso\Projecto\Pitstop-pro\Anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE72415-FDE0-4F61-95C8-62A5D2E014C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08417830-86E4-4BA2-8328-5193B62CF123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="56">
   <si>
     <t>Task</t>
   </si>
@@ -176,6 +176,18 @@
   </si>
   <si>
     <t>Tema inspirado nos sites de referência com cores Tailwind personalizadas</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Criar o layout da página e das funções que pretendo integrar.</t>
+  </si>
+  <si>
+    <t>Integrar o Firestore  para guardar eventos, manutenções, despesas etc</t>
   </si>
 </sst>
 </file>
@@ -613,13 +625,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomRight" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,7 +1106,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>48</v>
@@ -1105,6 +1117,35 @@
       <c r="E40" s="2" t="s">
         <v>49</v>
       </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="9"/>
+      <c r="E43" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat(garage): implement vehicle deletion with UI feedback and animation
- Added delete functionality to GarageVehicleCard with Firestore integration
- Replaced "Delete" text with Trash icon from Phosphor Icons
- Styled delete icon with hover effect and accessibility attributes (aria-label, title)
- Refactored GaragePage to pass loadVehicles callback for automatic UI refresh
- Maintained smooth animations on card entry using Framer Motion
</commit_message>
<xml_diff>
--- a/Anexos/pitstop_pro_taskboard.xlsx
+++ b/Anexos/pitstop_pro_taskboard.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kleman\OneDrive\Ambiente de Trabalho\Flag\Curso\Projecto\Pitstop-pro\Anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8873E9E-984C-4167-9CC6-06B6C5563B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB66B2AE-00B9-4831-B550-8FD4D3EC44A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="78">
   <si>
     <t>Task</t>
   </si>
@@ -248,6 +248,12 @@
   </si>
   <si>
     <t>Simula dados mock para visualização</t>
+  </si>
+  <si>
+    <t>Garage</t>
+  </si>
+  <si>
+    <t>Para tornar os frames mais interativos instalada dependência framer-motion</t>
   </si>
 </sst>
 </file>
@@ -354,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -381,7 +387,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,13 +691,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E49" sqref="E49"/>
+      <selection pane="bottomRight" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,7 +1170,7 @@
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>51</v>
       </c>
@@ -1359,6 +1364,39 @@
         <v>75</v>
       </c>
     </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
docs(taskboard): finalize and extend taskboard with completed and future tasks
</commit_message>
<xml_diff>
--- a/Anexos/pitstop_pro_taskboard.xlsx
+++ b/Anexos/pitstop_pro_taskboard.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kleman\OneDrive\Ambiente de Trabalho\Flag\Curso\Projecto\Pitstop-pro\Anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB66B2AE-00B9-4831-B550-8FD4D3EC44A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA2E61C-BC69-4B9F-9D73-DA9997AA8165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="122">
   <si>
     <t>Task</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Landing Page (Home)</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Estilo e UX</t>
   </si>
   <si>
@@ -169,9 +166,6 @@
     <t>repensar e aprofundar para aplicar melhor TS no que já existe.</t>
   </si>
   <si>
-    <t>Planed</t>
-  </si>
-  <si>
     <t>Tema inspirado nos sites de referência com cores Tailwind personalizadas</t>
   </si>
   <si>
@@ -254,6 +248,144 @@
   </si>
   <si>
     <t>Para tornar os frames mais interativos instalada dependência framer-motion</t>
+  </si>
+  <si>
+    <t>Mostra dados resumidos do veículo com foto, matrícula e botão de detalhes</t>
+  </si>
+  <si>
+    <t>Implementação de modais para criar e editar veículos</t>
+  </si>
+  <si>
+    <t>Adição da funcionalidade de eliminar veículos com confirmação</t>
+  </si>
+  <si>
+    <t>Organização visual dos cartões de veículo em grelha responsiva</t>
+  </si>
+  <si>
+    <t>Criação do tipo GarageVehicle em types/garageVehicle.ts</t>
+  </si>
+  <si>
+    <t>Estrutura base dos veículos com campos como brand, model, licensePlate, etc.</t>
+  </si>
+  <si>
+    <t>Criação do formulário GarageVehicleForm.tsx para criar e editar veículos</t>
+  </si>
+  <si>
+    <t>Criação do componente GarageVehicleCard.tsx para exibir dados do veículo</t>
+  </si>
+  <si>
+    <t>Integração da listagem de veículos na página MyGarage.tsx</t>
+  </si>
+  <si>
+    <t>Confirmação via window.confirm antes de apagar o documento no Firestore</t>
+  </si>
+  <si>
+    <t>Adição de dependência framer-motion para animações suaves nos cartões</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Criação da página Settings.tsx com estrutura base</t>
+  </si>
+  <si>
+    <t>Página estruturada com título, espaçamento e layout consistente com o resto da app</t>
+  </si>
+  <si>
+    <t>Criação do componente EditProfileSection.tsx</t>
+  </si>
+  <si>
+    <t>Permite editar campos opcionais como nome, morada, número de telemóvel e foto (URL)</t>
+  </si>
+  <si>
+    <t>Criação do componente ChangePasswordSection.tsx</t>
+  </si>
+  <si>
+    <t>Criação do componente DeleteAccountSection.tsx</t>
+  </si>
+  <si>
+    <t>Validação de campos opcionais no perfil</t>
+  </si>
+  <si>
+    <t>Estilização e layout responsivo dos componentes de Settings</t>
+  </si>
+  <si>
+    <t>Utiliza max-w-3xl e space-y com Tailwind para manter visual limpo e coerente</t>
+  </si>
+  <si>
+    <t>Criação de aviso na Navbar caso perfil esteja incompleto</t>
+  </si>
+  <si>
+    <t>Mostra alerta discreto a sugerir completar o perfil com link direto para Settings</t>
+  </si>
+  <si>
+    <t>Implementação de leitura e escrita dos dados de perfil no Firestore</t>
+  </si>
+  <si>
+    <t>Mensagens de loading (“Loading…”) para operações async?</t>
+  </si>
+  <si>
+    <t>Future Improvements</t>
+  </si>
+  <si>
+    <t>Implementar cálculo anual de despesas por veículo</t>
+  </si>
+  <si>
+    <t>Planned</t>
+  </si>
+  <si>
+    <t>Somar valores registados em Maintenance e Expenses por vehicleId e ano</t>
+  </si>
+  <si>
+    <t>Adicionar upload direto de documentos e faturas</t>
+  </si>
+  <si>
+    <t>Possível integração com Firebase Storage; atualmente é apenas via URL</t>
+  </si>
+  <si>
+    <t>Gerir consumos de combustível e portagens</t>
+  </si>
+  <si>
+    <t>Poderá ser feito com campos adicionais ou secções separadas por tipo de despesa</t>
+  </si>
+  <si>
+    <t>Adicionar suporte para modo claro/escuro (dark/light toggle)</t>
+  </si>
+  <si>
+    <t>Tailwind já tem suporte nativo com dark:; seria uma melhoria de UX</t>
+  </si>
+  <si>
+    <t>Criar seletor de idioma (i18n) para múltiplas línguas</t>
+  </si>
+  <si>
+    <t>Começar com en e pt, usando libs como react-i18next</t>
+  </si>
+  <si>
+    <t>Integrar APIs externas (seguros, inspeções, IMT, simuladores)</t>
+  </si>
+  <si>
+    <t>Abriria espaço a funcionalidades automáticas e dados em tempo real</t>
+  </si>
+  <si>
+    <t>Implementar notificações por e-mail/app sobre eventos futuros</t>
+  </si>
+  <si>
+    <t>Criar perfil de utilizador tipo “oficina” com painel dedicado</t>
+  </si>
+  <si>
+    <t>Explorar monetização por parcerias: oficinas, seguros, inspeções</t>
+  </si>
+  <si>
+    <t>Possibilidade de marcar revisões, simular seguros e incluir publicidade relevante</t>
+  </si>
+  <si>
+    <t>feito parcialmente** necessário rever</t>
+  </si>
+  <si>
+    <t>Firebase Functions + cron jobs ou outro tipo de soluções a pesquisar</t>
+  </si>
+  <si>
+    <t>Permite gestão de múltiplos veículos, visualização de clientes e agenda técnica, necessário repensar a aquitectura da app com os diferentes perfis</t>
   </si>
 </sst>
 </file>
@@ -282,7 +414,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,19 +435,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -360,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -374,17 +500,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -691,13 +814,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C64" sqref="C64"/>
+      <selection pane="bottomRight" activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,15 +842,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>19</v>
@@ -736,10 +859,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>19</v>
@@ -747,25 +870,25 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>42</v>
+      <c r="B4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -802,7 +925,7 @@
         <v>19</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -822,23 +945,23 @@
         <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -863,7 +986,7 @@
         <v>19</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -883,7 +1006,7 @@
         <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>19</v>
@@ -895,7 +1018,7 @@
         <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>19</v>
@@ -919,7 +1042,7 @@
         <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>19</v>
@@ -931,13 +1054,13 @@
         <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -945,7 +1068,7 @@
         <v>22</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>19</v>
@@ -953,20 +1076,20 @@
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>19</v>
@@ -1022,20 +1145,20 @@
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>19</v>
@@ -1059,7 +1182,7 @@
         <v>24</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>19</v>
@@ -1071,13 +1194,13 @@
         <v>24</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1105,297 +1228,649 @@
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>25</v>
+        <v>48</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>25</v>
+      <c r="D36" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>25</v>
+        <v>100</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
+      <c r="C39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E40" s="2"/>
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D41" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
+      <c r="C42" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E43" s="2"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>61</v>
-      </c>
+      <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
+      <c r="B50" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D54" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E54" s="2" t="s">
+      <c r="C57" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="1" t="s">
+      <c r="D57" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C56" s="1" t="s">
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E61" s="2"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D56" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E56" s="2"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="2"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="2"/>
+      <c r="D62" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" s="2"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E65" s="2"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="7"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E69" s="2"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" s="2"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E71" s="2"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B74" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E74" s="2"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="7"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B77" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B79" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B83" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>